<commit_message>
Created frontend for login page using find.css to style it. This CSS file was renamed to forms.css and altered to apply to any submission form pages, currently just the Find A Trail and Login pages. Backend was started on the login page to accept username and passwords. Some test users were entered into the "users" table in data.db, and a file called sql.py was created to test hashing functions and ways to validate hashed passwords with the database in a simpler environment with less variables before implementing it into the webapp. Functions to hash user passwords and validate entered passwords were created.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmons\Documents\Homework\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmons\Documents\Homework\Capstone\TrailFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9B037C-4E11-4B4C-98B8-6380E40364F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF148F16-68F3-4EE3-963F-BE158B256CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="6930" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="125">
   <si>
     <t>Team Members</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t xml:space="preserve">A TrailFinder logo was created using GIMP to trace a royalty-free image of a mountain biker, and Pixlr to put it together with text, shapes, and color. About an hour was spent on trying to add it to the navbar (this is still a work in progress at the moment). </t>
+  </si>
+  <si>
+    <t>Created frontend for login page using find.css to style it. This CSS file was renamed to forms.css and altered to apply to any submission form pages, currently just the Find A Trail and Login pages. Backend was started on the login page to accept username and passwords. Some test users were entered into the "users" table in data.db, and a file called sql.py was created to test hashing functions and ways to validate hashed passwords with the database in a simpler environment with less variables before implementing it into the webapp. Functions to hash user passwords and validate entered passwords were created.</t>
   </si>
 </sst>
 </file>
@@ -3093,8 +3096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3149,7 +3152,7 @@
       <c r="A3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="16">
         <v>45958</v>
       </c>
       <c r="C3" s="8">
@@ -3167,7 +3170,7 @@
       <c r="A4" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="16">
         <v>45959</v>
       </c>
       <c r="C4" s="8">
@@ -3217,14 +3220,22 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+    <row r="7" spans="1:6" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="16">
+        <v>45965</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
       <c r="D7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added user.py for future profile functionality.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="133">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t xml:space="preserve">I added a missing parameter (difficulty) to the frontend and backend of the Find A Trail page. Code was added to iterate through the database and grab parameters for each trail. Eventually this will be modified to only search trails within a certain radius to the entered location, but for now this works for getting the basics of the search feature working. Code was added to compare the parameters of each trail against the user-entered parameters, adding one point to it’s “trailscore” for each match. The results page was started with some minor CSS applied for styling, and backend to ensure that trails that passed the trailscore test are displayed (or a message letting the user know if there are no matching results) and ones that did not aren’t. Currently it is functional, though not nearly at the final version design-wise, it works for testing purposes. Additionally, a comment noting a test case that should yield no trail results was added to results.html for future reference when testing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Today consisted mostly of trying several ways to get user authentication to work in a way where, once someone logs in, they can stay logged in and have profile functionality. There was a lot of research and trial and error, but ultimately nothing worked well enough to stay in the code, which is why the only addition in GitHub is the user.py file. </t>
   </si>
 </sst>
 </file>
@@ -811,9 +814,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>232560</xdr:colOff>
+      <xdr:colOff>232200</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -823,7 +826,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6585120" cy="5052240"/>
+          <a:ext cx="6584760" cy="5051880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1034,9 +1037,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>169920</xdr:colOff>
+      <xdr:colOff>169560</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1046,7 +1049,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2565000" cy="714960"/>
+          <a:ext cx="2564640" cy="714600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1113,9 +1116,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>71280</xdr:colOff>
+      <xdr:colOff>70920</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:rowOff>26280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1125,7 +1128,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3725280" cy="15642000"/>
+          <a:ext cx="3724920" cy="15641640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1228,9 +1231,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>582840</xdr:colOff>
+      <xdr:colOff>582480</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1240,7 +1243,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3958200" cy="17462160"/>
+          <a:ext cx="3957840" cy="17461800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1487,9 +1490,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>90720</xdr:colOff>
+      <xdr:colOff>90360</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1499,7 +1502,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3510360" cy="15495480"/>
+          <a:ext cx="3510000" cy="15495120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2129,7 +2132,7 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3102,7 +3105,7 @@
   <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3315,14 +3318,20 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="22" t="n">
+        <v>45973</v>
+      </c>
+      <c r="C12" s="12" t="n">
+        <v>1.5</v>
+      </c>
       <c r="D12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>132</v>
+      </c>
       <c r="F12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Finished making images for the unfilled and filled bookmark icon. Redid some of the HTML for the Find A Trail results page, as well as the home.css file to make the results page look nicer and better organized. I then created trail difficulty icons and further modified the results page to display them next to the trail names.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -452,7 +452,22 @@
     <t xml:space="preserve">I added a missing parameter (difficulty) to the frontend and backend of the Find A Trail page. Code was added to iterate through the database and grab parameters for each trail. Eventually this will be modified to only search trails within a certain radius to the entered location, but for now this works for getting the basics of the search feature working. Code was added to compare the parameters of each trail against the user-entered parameters, adding one point to it’s “trailscore” for each match. The results page was started with some minor CSS applied for styling, and backend to ensure that trails that passed the trailscore test are displayed (or a message letting the user know if there are no matching results) and ones that did not aren’t. Currently it is functional, though not nearly at the final version design-wise, it works for testing purposes. Additionally, a comment noting a test case that should yield no trail results was added to results.html for future reference when testing.</t>
   </si>
   <si>
-    <t xml:space="preserve">Today consisted mostly of trying several ways to get user authentication to work in a way where, once someone logs in, they can stay logged in and have profile functionality. There was a lot of research and trial and error, but ultimately nothing worked well enough to stay in the code, which is why the only addition in GitHub is the user.py file. </t>
+    <t xml:space="preserve">SRCH.07, SRCH.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Today consisted mostly of trying several ways to get user authentication to work in a way where, once someone logs in, they can stay logged in and have profile functionality. There was a lot of research and trial and error, but ultimately nothing worked well enough to stay in the code, which is why the only addition in GitHub is the user.py file. Also, I went through some of the video filmed last week and marked file names and timestamps for parts I want to include to use for editing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVE.01, SRCH.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Began designing/learning how to design the graphic for the bookmark icon. Also began editing the video. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVE.01, SRCH.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished making images for the unfilled and filled bookmark icon. Redid some of the HTML for the Find A Trail results page, as well as the home.css file to make the results page look nicer and better organized. I then created trail difficulty icons and further modified the results page to display them next to the trail names. </t>
   </si>
 </sst>
 </file>
@@ -814,9 +829,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>232200</xdr:colOff>
+      <xdr:colOff>231120</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -826,7 +841,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6584760" cy="5051880"/>
+          <a:ext cx="6583680" cy="5050800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1037,9 +1052,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>169560</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>168480</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>184320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1049,7 +1064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2564640" cy="714600"/>
+          <a:ext cx="2563560" cy="713520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1116,9 +1131,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>70920</xdr:colOff>
+      <xdr:colOff>69840</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1128,7 +1143,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3724920" cy="15641640"/>
+          <a:ext cx="3723840" cy="15640560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1231,9 +1246,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>582480</xdr:colOff>
+      <xdr:colOff>581400</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1243,7 +1258,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3957840" cy="17461800"/>
+          <a:ext cx="3956760" cy="17460720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1490,9 +1505,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>90360</xdr:colOff>
+      <xdr:colOff>89280</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>97560</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1502,7 +1517,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3510000" cy="15495120"/>
+          <a:ext cx="3508920" cy="15494040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3105,7 +3120,7 @@
   <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3287,7 +3302,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="22" t="n">
-        <v>45965</v>
+        <v>45968</v>
       </c>
       <c r="C10" s="12" t="n">
         <v>1</v>
@@ -3318,40 +3333,58 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
+    <row r="12" customFormat="false" ht="117" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>132</v>
+      </c>
       <c r="B12" s="22" t="n">
         <v>45973</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="12"/>
+    <row r="13" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="22" t="n">
+        <v>45974</v>
+      </c>
+      <c r="C13" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="D13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="12"/>
+      <c r="E13" s="12" t="s">
+        <v>135</v>
+      </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="12"/>
+    <row r="14" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="22" t="n">
+        <v>45975</v>
+      </c>
+      <c r="C14" s="12" t="n">
+        <v>3</v>
+      </c>
       <c r="D14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="F14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
AddeI added functionality to calculate the distance between the user’s zip code and the zip code of the trail location. I then added a dropdown box that lets the user pick a distance to search in for trails. Now, trails will only show up as valid results if they are within the user-specified radius of their zip code. I tested this with several zip codes and distances to ensure it was working properly. I also made some minor adjustments to the CSS of the home page to prepare for adding the background video. d a to-do note in
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="141">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -468,6 +468,15 @@
   </si>
   <si>
     <t xml:space="preserve">Finished making images for the unfilled and filled bookmark icon. Redid some of the HTML for the Find A Trail results page, as well as the home.css file to make the results page look nicer and better organized. I then created trail difficulty icons and further modified the results page to display them next to the trail names. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I went out to get the last pieces of the footage I need for the main trail page. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRCH.04, SRCH.05, SRCH.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I added functionality to calculate the distance between the user’s zip code and the zip code of the trail location. I then added a dropdown box that lets the user pick a distance to search in for trails. Now, trails will only show up as valid results if they are within the user-specified radius of their zip code. I tested this with several zip codes and distances to ensure it was working properly. I also made some minor adjustments to the CSS of the home page to prepare for adding the background video. </t>
   </si>
 </sst>
 </file>
@@ -829,9 +838,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>231120</xdr:colOff>
+      <xdr:colOff>230400</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -841,7 +850,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6583680" cy="5050800"/>
+          <a:ext cx="6582960" cy="5050080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1052,9 +1061,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>168480</xdr:colOff>
+      <xdr:colOff>167760</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>184320</xdr:rowOff>
+      <xdr:rowOff>183600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1064,7 +1073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2563560" cy="713520"/>
+          <a:ext cx="2562840" cy="712800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1131,9 +1140,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>69840</xdr:colOff>
+      <xdr:colOff>69120</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1143,7 +1152,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3723840" cy="15640560"/>
+          <a:ext cx="3723120" cy="15639840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1246,9 +1255,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>581400</xdr:colOff>
+      <xdr:colOff>580680</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1258,7 +1267,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3956760" cy="17460720"/>
+          <a:ext cx="3956040" cy="17460000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1505,9 +1514,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>89280</xdr:colOff>
+      <xdr:colOff>88560</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1517,7 +1526,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3508920" cy="15494040"/>
+          <a:ext cx="3508200" cy="15493320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2147,7 +2156,7 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2842,7 +2851,7 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3119,8 +3128,8 @@
   </sheetPr>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3387,24 +3396,40 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="12"/>
+    <row r="15" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="22" t="n">
+        <v>45976</v>
+      </c>
+      <c r="C15" s="12" t="n">
+        <v>3</v>
+      </c>
       <c r="D15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>138</v>
+      </c>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="12"/>
+    <row r="16" customFormat="false" ht="117" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="22" t="n">
+        <v>45980</v>
+      </c>
+      <c r="C16" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="D16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="12" t="s">
+        <v>140</v>
+      </c>
       <c r="F16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
I went through the footage from 11/15 to make the final decisions on what will be included in the video. Then I had to spend some time troubleshooting several of the video files not appearing in the video editing software, ultimately having to convert the codecs of the videos. Once this was done, I cut out the unnecessary parts of the clips, decided their order, color corrected the clips, and rendered the video to an MP4 file that can be played in a webpage. Next, the video was added to the home page in home.html, and home.css was adjusted to give it a proper layout and lower opacity so the TrailFinder welcome message can still be seen over it. I tested it on multiple displays and found the video did not appear properly on 4K displays, so I adjusted the CSS further until it displayed properly on both 1080p and 4K displays. I also tried changing my monitor resolution to various other options and confirmed that it worked on those as well.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="142">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t xml:space="preserve">I added functionality to calculate the distance between the user’s zip code and the zip code of the trail location. I then added a dropdown box that lets the user pick a distance to search in for trails. Now, trails will only show up as valid results if they are within the user-specified radius of their zip code. I tested this with several zip codes and distances to ensure it was working properly. I also made some minor adjustments to the CSS of the home page to prepare for adding the background video. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I went through the footage from 11/15 to make the final decisions on what will be included in the video. Then I had to spend some time troubleshooting several of the video files not appearing in the video editing software, ultimately having to convert the codecs of the videos. Once this was done, I cut out the unnecessary parts of the clips, decided their order, color corrected the clips, and rendered the video to an MP4 file that can be played in a webpage. Next, the video was added to the home page in home.html, and home.css was adjusted to give it a proper layout and lower opacity so the TrailFinder welcome message can still be seen over it. I tested it on multiple displays and found the video did not appear properly on 4K displays, so I adjusted the CSS further until it displayed properly on both 1080p and 4K displays. I also tried changing my monitor resolution to various other options and confirmed that it worked on those as well. </t>
   </si>
 </sst>
 </file>
@@ -838,9 +841,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>230400</xdr:colOff>
+      <xdr:colOff>230040</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -850,7 +853,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6582960" cy="5050080"/>
+          <a:ext cx="6582600" cy="5049720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1061,9 +1064,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>167760</xdr:colOff>
+      <xdr:colOff>167400</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>183600</xdr:rowOff>
+      <xdr:rowOff>183240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1073,7 +1076,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2562840" cy="712800"/>
+          <a:ext cx="2562480" cy="712440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1140,9 +1143,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>69120</xdr:colOff>
+      <xdr:colOff>68760</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1152,7 +1155,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3723120" cy="15639840"/>
+          <a:ext cx="3722760" cy="15639480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1255,9 +1258,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>580680</xdr:colOff>
+      <xdr:colOff>580320</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1267,7 +1270,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3956040" cy="17460000"/>
+          <a:ext cx="3955680" cy="17459640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1514,9 +1517,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>88560</xdr:colOff>
+      <xdr:colOff>88200</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1526,7 +1529,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3508200" cy="15493320"/>
+          <a:ext cx="3507840" cy="15492960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3129,7 +3132,7 @@
   <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3432,14 +3435,22 @@
       </c>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="12"/>
+    <row r="17" customFormat="false" ht="220.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="22" t="n">
+        <v>45981</v>
+      </c>
+      <c r="C17" s="12" t="n">
+        <v>2.5</v>
+      </c>
       <c r="D17" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="12" t="s">
+        <v>141</v>
+      </c>
       <c r="F17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
I adjusted the find_a_trail function in main.py and the results.html file to display different alt text for each difficulty rating icon that could appear in the search results. I tested this by performing a search that showed at least one trail from each difficulty, then I checked the image’s properties using the inspect tool to ensure the alt text was showing up correctly. I completed the User object in user.py, and began implementing functions to check if a user is logged in. If they are, instead of the register or login buttons, there is a logout button on the home page. Additionally, I adjusted the register function in main.py so when a user registers they are automatically logged in (if the username doesn’t already exist).
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="143">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -480,6 +480,9 @@
   </si>
   <si>
     <t xml:space="preserve">I went through the footage from 11/15 to make the final decisions on what will be included in the video. Then I had to spend some time troubleshooting several of the video files not appearing in the video editing software, ultimately having to convert the codecs of the videos. Once this was done, I cut out the unnecessary parts of the clips, decided their order, color corrected the clips, and rendered the video to an MP4 file that can be played in a webpage. Next, the video was added to the home page in home.html, and home.css was adjusted to give it a proper layout and lower opacity so the TrailFinder welcome message can still be seen over it. I tested it on multiple displays and found the video did not appear properly on 4K displays, so I adjusted the CSS further until it displayed properly on both 1080p and 4K displays. I also tried changing my monitor resolution to various other options and confirmed that it worked on those as well. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I adjusted the find_a_trail function in main.py and the results.html file to display different alt text for each difficulty rating icon that could appear in the search results. I tested this by performing a search that showed at least one trail from each difficulty, then I checked the image’s properties using the inspect tool to ensure the alt text was showing up correctly. I completed the User object in user.py, and began implementing functions to check if a user is logged in. If they are, instead of the register or login buttons, there is a logout button on the home page. Additionally, I adjusted the register function in main.py so when a user registers they are automatically logged in (if the username doesn’t already exist). </t>
   </si>
 </sst>
 </file>
@@ -841,9 +844,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>230040</xdr:colOff>
+      <xdr:colOff>229680</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -853,7 +856,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6582600" cy="5049720"/>
+          <a:ext cx="6582240" cy="5049360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1064,9 +1067,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>167400</xdr:colOff>
+      <xdr:colOff>167040</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1076,7 +1079,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2562480" cy="712440"/>
+          <a:ext cx="2562120" cy="712080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1143,9 +1146,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>68760</xdr:colOff>
+      <xdr:colOff>68400</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1155,7 +1158,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3722760" cy="15639480"/>
+          <a:ext cx="3722400" cy="15639120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1258,9 +1261,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>580320</xdr:colOff>
+      <xdr:colOff>579960</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1270,7 +1273,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3955680" cy="17459640"/>
+          <a:ext cx="3955320" cy="17459280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1517,9 +1520,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>88200</xdr:colOff>
+      <xdr:colOff>87840</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1529,7 +1532,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3507840" cy="15492960"/>
+          <a:ext cx="3507480" cy="15492600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3131,8 +3134,8 @@
   </sheetPr>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3453,14 +3456,22 @@
       </c>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="12"/>
+    <row r="18" customFormat="false" ht="174.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="22" t="n">
+        <v>45982</v>
+      </c>
+      <c r="C18" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D18" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="12" t="s">
+        <v>142</v>
+      </c>
       <c r="F18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
I added an error message functionality to the register page for when someone attempts to sign up with a username that already exists. I also added error message functionality for the login page, which will show an error for an incorrect password and for a username that doesn’t exist. It is set up so any future errors just need to be passed to the HTML file and will show up without having to edit any HTML or CSS. The forms.css file was modified to include styling for the error messages.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="144">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -483,6 +483,9 @@
   </si>
   <si>
     <t xml:space="preserve">I adjusted the find_a_trail function in main.py and the results.html file to display different alt text for each difficulty rating icon that could appear in the search results. I tested this by performing a search that showed at least one trail from each difficulty, then I checked the image’s properties using the inspect tool to ensure the alt text was showing up correctly. I completed the User object in user.py, and began implementing functions to check if a user is logged in. If they are, instead of the register or login buttons, there is a logout button on the home page. Additionally, I adjusted the register function in main.py so when a user registers they are automatically logged in (if the username doesn’t already exist). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I added an error message functionality to the register page for when someone attempts to sign up with a username that already exists. I also added error message functionality for the login page, which will show an error for an incorrect password and for a username that doesn’t exist. It is set up so any future errors just need to be passed to the HTML file and will show up without having to edit any HTML or CSS. The forms.css file was modified to include styling for the error messages. </t>
   </si>
 </sst>
 </file>
@@ -844,9 +847,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>229680</xdr:colOff>
+      <xdr:colOff>229320</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -856,7 +859,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6582240" cy="5049360"/>
+          <a:ext cx="6581880" cy="5049000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1067,9 +1070,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>167040</xdr:colOff>
+      <xdr:colOff>166680</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:rowOff>182520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1079,7 +1082,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2562120" cy="712080"/>
+          <a:ext cx="2561760" cy="711720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1146,9 +1149,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>68400</xdr:colOff>
+      <xdr:colOff>68040</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>23760</xdr:rowOff>
+      <xdr:rowOff>23400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1158,7 +1161,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3722400" cy="15639120"/>
+          <a:ext cx="3722040" cy="15638760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1261,9 +1264,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>579960</xdr:colOff>
+      <xdr:colOff>579600</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1273,7 +1276,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3955320" cy="17459280"/>
+          <a:ext cx="3954960" cy="17458920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1520,9 +1523,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>87840</xdr:colOff>
+      <xdr:colOff>87480</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1532,7 +1535,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3507480" cy="15492600"/>
+          <a:ext cx="3507120" cy="15492240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2162,7 +2165,7 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3134,8 +3137,8 @@
   </sheetPr>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3474,14 +3477,22 @@
       </c>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="12"/>
+    <row r="19" customFormat="false" ht="117" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="22" t="n">
+        <v>45985</v>
+      </c>
+      <c r="C19" s="12" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="F19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
A new table in the database called preference was created that will keep track of the number of times a user selects each of the options in the terrain, type, and difficulty dropboxes on the Find A Trail page. I cleaned up some unnecessary code where I created more cursors for accessing the database than was necessary. I also began writing code to automatically create an entry in the preference table for a user when they register. This unfortunately took a lot of time due to some trouble with SQLite3’s syntax and unspecific error output. I then wrote a script (user_update.py) to insert the existing users into the preference table, which also took longer than it should have due to the same reasons. Finally, I created the update_prefs function in main.py to update the preferences table. Then I spent more time troubleshooting that function since SQLite’s syntax is once again giving me trouble… But that’s tomorrow’s problem.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="145">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t xml:space="preserve">I added an error message functionality to the register page for when someone attempts to sign up with a username that already exists. I also added error message functionality for the login page, which will show an error for an incorrect password and for a username that doesn’t exist. It is set up so any future errors just need to be passed to the HTML file and will show up without having to edit any HTML or CSS. The forms.css file was modified to include styling for the error messages. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new table in the database called preference was created that will keep track of the number of times a user selects each of the options in the terrain, type, and difficulty dropboxes on the Find A Trail page. I cleaned up some unnecessary code where I created more cursors for accessing the database than was necessary. I also began writing code to automatically create an entry in the preference table for a user when they register. This unfortunately took a lot of time due to some trouble with SQLite3’s syntax and unspecific error output. I then wrote a script (user_update.py) to insert the existing users into the preference table, which also took longer than it should have due to the same reasons. Finally, I created the update_prefs function in main.py to update the preferences table. Then I spent more time troubleshooting that function since SQLite’s syntax is once again giving me trouble… But that’s tomorrow’s problem. </t>
   </si>
 </sst>
 </file>
@@ -847,9 +850,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>229320</xdr:colOff>
+      <xdr:colOff>228960</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -859,7 +862,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6581880" cy="5049000"/>
+          <a:ext cx="6581520" cy="5048640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1070,9 +1073,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>166680</xdr:colOff>
+      <xdr:colOff>166320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>182520</xdr:rowOff>
+      <xdr:rowOff>182160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1082,7 +1085,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2561760" cy="711720"/>
+          <a:ext cx="2561400" cy="711360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1149,9 +1152,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>68040</xdr:colOff>
+      <xdr:colOff>67680</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1161,7 +1164,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3722040" cy="15638760"/>
+          <a:ext cx="3721680" cy="15638400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1264,9 +1267,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>579600</xdr:colOff>
+      <xdr:colOff>579240</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1276,7 +1279,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3954960" cy="17458920"/>
+          <a:ext cx="3954600" cy="17458560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1523,9 +1526,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>87480</xdr:colOff>
+      <xdr:colOff>87120</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1535,7 +1538,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3507120" cy="15492240"/>
+          <a:ext cx="3506760" cy="15491880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2165,8 +2168,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3138,7 +3141,7 @@
   <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3495,14 +3498,22 @@
       </c>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="12"/>
+    <row r="20" customFormat="false" ht="220.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="22" t="n">
+        <v>45986</v>
+      </c>
+      <c r="C20" s="12" t="n">
+        <v>2.5</v>
+      </c>
       <c r="D20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>144</v>
+      </c>
       <c r="F20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
I fixed the database update issues when trying to store the users preferences in the preference table. I tested it with a few searches logged in as testuser1 and confirmed that the correct entries update in the table. I also did some general code cleanup, like switching fetchall() calls to fetchone() when only one variable was being searched for in a database query and cleaning up/adding comments to better document the code. I also changed the login function to redirect to home on successful login, rather than just pull up the home HTML file, since that caused the browser to display the URL for login when first redirected to the home page after logging in.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="146">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -489,6 +489,9 @@
   </si>
   <si>
     <t xml:space="preserve">A new table in the database called preference was created that will keep track of the number of times a user selects each of the options in the terrain, type, and difficulty dropboxes on the Find A Trail page. I cleaned up some unnecessary code where I created more cursors for accessing the database than was necessary. I also began writing code to automatically create an entry in the preference table for a user when they register. This unfortunately took a lot of time due to some trouble with SQLite3’s syntax and unspecific error output. I then wrote a script (user_update.py) to insert the existing users into the preference table, which also took longer than it should have due to the same reasons. Finally, I created the update_prefs function in main.py to update the preferences table. Then I spent more time troubleshooting that function since SQLite’s syntax is once again giving me trouble… But that’s tomorrow’s problem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I fixed the database update issues when trying to store the users preferences in the preference table. I tested it with a few searches logged in as testuser1 and confirmed that the correct entries update in the table. I also did some general code cleanup, like switching fetchall() calls to fetchone() when only one variable was being searched for in a database query and cleaning up/adding comments to better document the code. I also changed the login function to redirect to home on successful login, rather than just pull up the home HTML file, since that caused the browser to display the URL for login when first redirected to the home page after logging in. </t>
   </si>
 </sst>
 </file>
@@ -850,9 +853,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -862,7 +865,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6581520" cy="5048640"/>
+          <a:ext cx="6581160" cy="5048280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1073,9 +1076,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>166320</xdr:colOff>
+      <xdr:colOff>165960</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>182160</xdr:rowOff>
+      <xdr:rowOff>181800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1085,7 +1088,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2561400" cy="711360"/>
+          <a:ext cx="2561040" cy="711000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1152,9 +1155,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>67680</xdr:colOff>
+      <xdr:colOff>67320</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>23040</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1164,7 +1167,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3721680" cy="15638400"/>
+          <a:ext cx="3721320" cy="15638040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1267,9 +1270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>579240</xdr:colOff>
+      <xdr:colOff>578880</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1279,7 +1282,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3954600" cy="17458560"/>
+          <a:ext cx="3954240" cy="17458200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1526,9 +1529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>87120</xdr:colOff>
+      <xdr:colOff>86760</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>93960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1538,7 +1541,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3506760" cy="15491880"/>
+          <a:ext cx="3506400" cy="15491520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3140,8 +3143,8 @@
   </sheetPr>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3516,14 +3519,22 @@
       </c>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="12"/>
+    <row r="21" customFormat="false" ht="151.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="22" t="n">
+        <v>45987</v>
+      </c>
+      <c r="C21" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="D21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="12" t="s">
+        <v>145</v>
+      </c>
       <c r="F21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
I fixed an issue that caused an exception to be thrown whenever the logout button was used. I think tested searching for trails a few times, logged in as various test users, and logged out, to confirm that the logout function was working properly. I also fixed a similar URL error as yesterday, this time with the logout URL appearing on the home page after logging out. I created an HTML file called not_logged.html and set it up to display if a user selects the Recommend A Trail or Saved Trails buttons, showing them that they need to be logged in to use those features, and providing a link to do so. I began researching how to implement the save button into the results page, specifically how to make a button with an image that can change on click. It appears JavaScript may be needed for that. I also began adding in the backend functionality for the Recommend A Trail feature.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="149">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -491,7 +491,16 @@
     <t xml:space="preserve">A new table in the database called preference was created that will keep track of the number of times a user selects each of the options in the terrain, type, and difficulty dropboxes on the Find A Trail page. I cleaned up some unnecessary code where I created more cursors for accessing the database than was necessary. I also began writing code to automatically create an entry in the preference table for a user when they register. This unfortunately took a lot of time due to some trouble with SQLite3’s syntax and unspecific error output. I then wrote a script (user_update.py) to insert the existing users into the preference table, which also took longer than it should have due to the same reasons. Finally, I created the update_prefs function in main.py to update the preferences table. Then I spent more time troubleshooting that function since SQLite’s syntax is once again giving me trouble… But that’s tomorrow’s problem. </t>
   </si>
   <si>
+    <t xml:space="preserve">RECS.01, SRCH.02</t>
+  </si>
+  <si>
     <t xml:space="preserve">I fixed the database update issues when trying to store the users preferences in the preference table. I tested it with a few searches logged in as testuser1 and confirmed that the correct entries update in the table. I also did some general code cleanup, like switching fetchall() calls to fetchone() when only one variable was being searched for in a database query and cleaning up/adding comments to better document the code. I also changed the login function to redirect to home on successful login, rather than just pull up the home HTML file, since that caused the browser to display the URL for login when first redirected to the home page after logging in. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRCH.02, SRCH.07, RECS.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I fixed an issue that caused an exception to be thrown whenever the logout button was used. I think tested searching for trails a few times, logged in as various test users, and logged out, to confirm that the logout function was working properly. I also fixed a similar URL error as yesterday, this time with the logout URL appearing on the home page after logging out. I created an HTML file called not_logged.html and set it up to display if a user selects the Recommend A Trail or Saved Trails buttons, showing them that they need to be logged in to use those features, and providing a link to do so. I began researching how to implement the save button into the results page, specifically how to make a button with an image that can change on click. It appears JavaScript may be needed for that. I also began adding in the backend functionality for the Recommend A Trail feature. </t>
   </si>
 </sst>
 </file>
@@ -853,9 +862,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228240</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -865,7 +874,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6581160" cy="5048280"/>
+          <a:ext cx="6580800" cy="5047920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1076,9 +1085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>165960</xdr:colOff>
+      <xdr:colOff>165600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1088,7 +1097,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2561040" cy="711000"/>
+          <a:ext cx="2560680" cy="710640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1155,9 +1164,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>67320</xdr:colOff>
+      <xdr:colOff>66960</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1167,7 +1176,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3721320" cy="15638040"/>
+          <a:ext cx="3720960" cy="15637680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1270,9 +1279,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>578880</xdr:colOff>
+      <xdr:colOff>578520</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1282,7 +1291,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3954240" cy="17458200"/>
+          <a:ext cx="3953880" cy="17457840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1529,9 +1538,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>86760</xdr:colOff>
+      <xdr:colOff>86400</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1541,7 +1550,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3506400" cy="15491520"/>
+          <a:ext cx="3506040" cy="15491160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2171,7 +2180,7 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -3143,8 +3152,8 @@
   </sheetPr>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3521,7 +3530,7 @@
     </row>
     <row r="21" customFormat="false" ht="151.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="B21" s="22" t="n">
         <v>45987</v>
@@ -3533,18 +3542,26 @@
         <v>33</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="12"/>
+    <row r="22" customFormat="false" ht="209" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="22" t="n">
+        <v>45989</v>
+      </c>
+      <c r="C22" s="12" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="12" t="s">
+        <v>148</v>
+      </c>
       <c r="F22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
I set up the database queries to get trails that match the user preferences.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="150">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t xml:space="preserve">I fixed an issue that caused an exception to be thrown whenever the logout button was used. I think tested searching for trails a few times, logged in as various test users, and logged out, to confirm that the logout function was working properly. I also fixed a similar URL error as yesterday, this time with the logout URL appearing on the home page after logging out. I created an HTML file called not_logged.html and set it up to display if a user selects the Recommend A Trail or Saved Trails buttons, showing them that they need to be logged in to use those features, and providing a link to do so. I began researching how to implement the save button into the results page, specifically how to make a button with an image that can change on click. It appears JavaScript may be needed for that. I also began adding in the backend functionality for the Recommend A Trail feature. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I set up the database queries to get trails that match the user preferences. </t>
   </si>
 </sst>
 </file>
@@ -862,9 +865,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>228240</xdr:colOff>
+      <xdr:colOff>227880</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -874,7 +877,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6580800" cy="5047920"/>
+          <a:ext cx="6580440" cy="5047560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1085,9 +1088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>165600</xdr:colOff>
+      <xdr:colOff>165240</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1097,7 +1100,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2560680" cy="710640"/>
+          <a:ext cx="2560320" cy="710280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1164,9 +1167,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>66960</xdr:colOff>
+      <xdr:colOff>66600</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1176,7 +1179,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3720960" cy="15637680"/>
+          <a:ext cx="3720600" cy="15637320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1279,9 +1282,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>578520</xdr:colOff>
+      <xdr:colOff>578160</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1291,7 +1294,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3953880" cy="17457840"/>
+          <a:ext cx="3953520" cy="17457480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1538,9 +1541,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>86400</xdr:colOff>
+      <xdr:colOff>86040</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>93600</xdr:rowOff>
+      <xdr:rowOff>93240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1550,7 +1553,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3506040" cy="15491160"/>
+          <a:ext cx="3505680" cy="15490800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3153,7 +3156,7 @@
   <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3564,14 +3567,22 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="12"/>
+    <row r="23" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="22" t="n">
+        <v>45991</v>
+      </c>
+      <c r="C23" s="12" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>149</v>
+      </c>
       <c r="F23" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
I renamed rec.html to recs.html to fit better with the naming conventions used throughout other portions of the project. I copied the HTML from results.html to rec.html, then spent awhile debugging the Python code written yesterday when attempting to test the recommendations feature, and then some more time modifying the HTML to better fit this specific page, which included editing the header, the trail information that actually displays (and some of the Python code for how to display it), and adding a note explaining how the feature works.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="152">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t xml:space="preserve">I set up the database queries to get trails that match the user preferences. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECS.02, RECS.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I renamed rec.html to recs.html to fit better with the naming conventions used throughout other portions of the project. I copied the HTML from results.html to rec.html, then spent awhile debugging the Python code written yesterday when attempting to test the recommendations feature, and then some more time modifying the HTML to better fit this specific page, which included editing the header, the trail information that actually displays (and some of the Python code for how to display it), and adding a note explaining how the feature works. </t>
   </si>
 </sst>
 </file>
@@ -865,9 +871,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>227880</xdr:colOff>
+      <xdr:colOff>227520</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -877,7 +883,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6580440" cy="5047560"/>
+          <a:ext cx="6580080" cy="5047200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1088,9 +1094,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>165240</xdr:colOff>
+      <xdr:colOff>164880</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>181080</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1100,7 +1106,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2560320" cy="710280"/>
+          <a:ext cx="2559960" cy="709920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1167,9 +1173,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>66600</xdr:colOff>
+      <xdr:colOff>66240</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1179,7 +1185,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3720600" cy="15637320"/>
+          <a:ext cx="3720240" cy="15636960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1282,9 +1288,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>578160</xdr:colOff>
+      <xdr:colOff>577800</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1294,7 +1300,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3953520" cy="17457480"/>
+          <a:ext cx="3953160" cy="17457120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1541,9 +1547,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>86040</xdr:colOff>
+      <xdr:colOff>85680</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>93240</xdr:rowOff>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1553,7 +1559,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3505680" cy="15490800"/>
+          <a:ext cx="3505320" cy="15490440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2183,8 +2189,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3156,7 +3162,7 @@
   <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3585,14 +3591,22 @@
       </c>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="12"/>
+    <row r="24" customFormat="false" ht="128.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" s="22" t="n">
+        <v>45992</v>
+      </c>
+      <c r="C24" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="D24" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="12" t="s">
+        <v>151</v>
+      </c>
       <c r="F24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
I went through and cleaned up some print statements that I had used for testing purposes but didn’t need anymore to make both the code and terminal output cleaner. I also created results.css to use for the results.html and recs.html pages, since the styling needs for this project have grown to a point where keeping the majority of it in one shared CSS file is becoming complicated and introducing issues. I then was able to set up the bookmark button on the results page for finding a trail, as well as the hover effect. I then created a JavaScript file to handle the button’s image changing on click, and spent about half of today’s work time trying to figure out why the file wouldn’t link, which is an issue I have not successfully solved yet.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="153">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -510,6 +510,9 @@
   </si>
   <si>
     <t xml:space="preserve">I renamed rec.html to recs.html to fit better with the naming conventions used throughout other portions of the project. I copied the HTML from results.html to rec.html, then spent awhile debugging the Python code written yesterday when attempting to test the recommendations feature, and then some more time modifying the HTML to better fit this specific page, which included editing the header, the trail information that actually displays (and some of the Python code for how to display it), and adding a note explaining how the feature works. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I went through and cleaned up some print statements that I had used for testing purposes but didn’t need anymore to make both the code and terminal output cleaner. I also created results.css to use for the results.html and recs.html pages, since the styling needs for this project have grown to a point where keeping the majority of it in one shared CSS file is becoming complicated and introducing issues. I then was able to set up the bookmark button on the results page for finding a trail, as well as the hover effect. I then created a JavaScript file to handle the button’s image changing on click, and spent about half of today’s work time trying to figure out why the file wouldn’t link, which is an issue I have not successfully solved yet. </t>
   </si>
 </sst>
 </file>
@@ -871,9 +874,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>227520</xdr:colOff>
+      <xdr:colOff>227160</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -883,7 +886,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6580080" cy="5047200"/>
+          <a:ext cx="6579720" cy="5046840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1094,9 +1097,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>164880</xdr:colOff>
+      <xdr:colOff>164520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1106,7 +1109,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2559960" cy="709920"/>
+          <a:ext cx="2559600" cy="709560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1173,9 +1176,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>66240</xdr:colOff>
+      <xdr:colOff>65880</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1185,7 +1188,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3720240" cy="15636960"/>
+          <a:ext cx="3719880" cy="15636600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1288,9 +1291,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>577800</xdr:colOff>
+      <xdr:colOff>577440</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1300,7 +1303,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3953160" cy="17457120"/>
+          <a:ext cx="3952800" cy="17456760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1547,9 +1550,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>85680</xdr:colOff>
+      <xdr:colOff>85320</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
+      <xdr:rowOff>92520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1559,7 +1562,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3505320" cy="15490440"/>
+          <a:ext cx="3504960" cy="15490080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2190,7 +2193,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3161,8 +3164,8 @@
   </sheetPr>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3609,14 +3612,20 @@
       </c>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="174.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="12"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="12"/>
+      <c r="B25" s="22" t="n">
+        <v>45993</v>
+      </c>
+      <c r="C25" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D25" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="12" t="s">
+        <v>152</v>
+      </c>
       <c r="F25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
I did some more research and troubleshooting on the JS file issue, with no luck. I then set up some test data in the notes table to proceed with setting up the backend for the saved trails while troubleshooting the issue, and begin on the notes feature. I set up the saved_trails function in main.py and the saved.html file to display saved trails and notes for those trails. I then created saved.py to create backend for a text box and the save and cancel buttons so the user can enter in notes. I then adjusted saved.html to display the notes field and results.css to style it. I tried to get existing notes to appear and be editable in the WTForms TextArea field, but could not, so for now I have it set up to display existing notes above the notes section. I did some research into a custom WTForms widget to fix this, but it is lower priority at the moment while I get the full functionality finished.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="156">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -512,7 +512,16 @@
     <t xml:space="preserve">I renamed rec.html to recs.html to fit better with the naming conventions used throughout other portions of the project. I copied the HTML from results.html to rec.html, then spent awhile debugging the Python code written yesterday when attempting to test the recommendations feature, and then some more time modifying the HTML to better fit this specific page, which included editing the header, the trail information that actually displays (and some of the Python code for how to display it), and adding a note explaining how the feature works. </t>
   </si>
   <si>
+    <t xml:space="preserve">SAVE.01, SAVE.02</t>
+  </si>
+  <si>
     <t xml:space="preserve">I went through and cleaned up some print statements that I had used for testing purposes but didn’t need anymore to make both the code and terminal output cleaner. I also created results.css to use for the results.html and recs.html pages, since the styling needs for this project have grown to a point where keeping the majority of it in one shared CSS file is becoming complicated and introducing issues. I then was able to set up the bookmark button on the results page for finding a trail, as well as the hover effect. I then created a JavaScript file to handle the button’s image changing on click, and spent about half of today’s work time trying to figure out why the file wouldn’t link, which is an issue I have not successfully solved yet. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVE.02, SAVE.03, SAVE.04, NOTE.01, NOTE.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I did some more research and troubleshooting on the JS file issue, with no luck. I then set up some test data in the notes table to proceed with setting up the backend for the saved trails while troubleshooting the issue, and begin on the notes feature. I set up the saved_trails function in main.py and the saved.html file to display saved trails and notes for those trails. I then created saved.py to create backend for a text box and the save and cancel buttons so the user can enter in notes. I then adjusted saved.html to display the notes field and results.css to style it. I tried to get existing notes to appear and be editable in the WTForms TextArea field, but could not, so for now I have it set up to display existing notes above the notes section. I did some research into a custom WTForms widget to fix this, but it is lower priority at the moment while I get the full functionality finished.</t>
   </si>
 </sst>
 </file>
@@ -874,9 +883,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>227160</xdr:colOff>
+      <xdr:colOff>226800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -886,7 +895,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6579720" cy="5046840"/>
+          <a:ext cx="6579360" cy="5046480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1097,9 +1106,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>164520</xdr:colOff>
+      <xdr:colOff>164160</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1109,7 +1118,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2559600" cy="709560"/>
+          <a:ext cx="2559240" cy="709200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1176,9 +1185,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1188,7 +1197,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3719880" cy="15636600"/>
+          <a:ext cx="3719520" cy="15636240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1291,9 +1300,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>577440</xdr:colOff>
+      <xdr:colOff>577080</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1303,7 +1312,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3952800" cy="17456760"/>
+          <a:ext cx="3952440" cy="17456400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1550,9 +1559,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1562,7 +1571,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3504960" cy="15490080"/>
+          <a:ext cx="3504600" cy="15489720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2066,7 +2075,7 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -3164,7 +3173,7 @@
   </sheetPr>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -3613,7 +3622,9 @@
       <c r="F24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="174.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12"/>
+      <c r="A25" s="12" t="s">
+        <v>152</v>
+      </c>
       <c r="B25" s="22" t="n">
         <v>45993</v>
       </c>
@@ -3624,18 +3635,26 @@
         <v>33</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="12"/>
+    <row r="26" customFormat="false" ht="209" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="22" t="n">
+        <v>45994</v>
+      </c>
+      <c r="C26" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D26" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="F26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Partial push for the day
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="158">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t xml:space="preserve">I did some more research and troubleshooting on the JS file issue, with no luck. I then set up some test data in the notes table to proceed with setting up the backend for the saved trails while troubleshooting the issue, and begin on the notes feature. I set up the saved_trails function in main.py and the saved.html file to display saved trails and notes for those trails. I then created saved.py to create backend for a text box and the save and cancel buttons so the user can enter in notes. I then adjusted saved.html to display the notes field and results.css to style it. I tried to get existing notes to appear and be editable in the WTForms TextArea field, but could not, so for now I have it set up to display existing notes above the notes section. I did some research into a custom WTForms widget to fix this, but it is lower priority at the moment while I get the full functionality finished.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVE.02, SAVE.03, SAVE.04, NOTE.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I moved the main.js file to the static folder, and the terminal no longer throws a 404 when trying to load it. However, the JS function still does not execute, so I spent some time researching and debugging that issue. I eventually found that the JavaScript file was including the full domain as the image source (starting with http://(my domain), and changed the if statement to check if the source ended with the file path, rather than if it was equal to it, which fixed the issue. However, selecting the save icon on any trail will only fill the icon for the first trail displayed, which I did some research on solutions for, and will continue to work on later. I edited saved.html to display a message when a logged in user has no saved trails informing them of that. I then started researching ways to get the trail data necessary to upload notes for a specific trail when the user clicks the save button. This is difficult because the trails are displayed with a for loop, and therefore do not have unique IDs to get them from the HTML by. I spent some time trying to set the save buttons to give them an ID name that matches the trail name to use that for updating the database.</t>
   </si>
 </sst>
 </file>
@@ -883,9 +889,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>226800</xdr:colOff>
+      <xdr:colOff>226440</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -895,7 +901,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6579360" cy="5046480"/>
+          <a:ext cx="6579000" cy="5046120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1106,9 +1112,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>164160</xdr:colOff>
+      <xdr:colOff>163800</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>180000</xdr:rowOff>
+      <xdr:rowOff>179640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1118,7 +1124,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2559240" cy="709200"/>
+          <a:ext cx="2558880" cy="708840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1185,9 +1191,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>65520</xdr:colOff>
+      <xdr:colOff>65160</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1197,7 +1203,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3719520" cy="15636240"/>
+          <a:ext cx="3719160" cy="15635880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1300,9 +1306,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>577080</xdr:colOff>
+      <xdr:colOff>576720</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1312,7 +1318,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3952440" cy="17456400"/>
+          <a:ext cx="3952080" cy="17456040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1559,9 +1565,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>92160</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1571,7 +1577,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3504600" cy="15489720"/>
+          <a:ext cx="3504240" cy="15489360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2075,7 +2081,7 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2896,8 +2902,8 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3173,8 +3179,8 @@
   </sheetPr>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3657,14 +3663,22 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="12"/>
+    <row r="27" customFormat="false" ht="266.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="22" t="n">
+        <v>45995</v>
+      </c>
+      <c r="C27" s="12" t="n">
+        <v>1.75</v>
+      </c>
       <c r="D27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="12" t="s">
+        <v>157</v>
+      </c>
       <c r="F27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
The database and workbook didn't get properly uploaded to GitHub, adding the correct versions here.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -527,7 +527,7 @@
     <t xml:space="preserve">SAVE.02, SAVE.03, SAVE.04, NOTE.02</t>
   </si>
   <si>
-    <t xml:space="preserve">I moved the main.js file to the static folder, and the terminal no longer throws a 404 when trying to load it. However, the JS function still does not execute, so I spent some time researching and debugging that issue. I eventually found that the JavaScript file was including the full domain as the image source (starting with http://(my domain), and changed the if statement to check if the source ended with the file path, rather than if it was equal to it, which fixed the issue. However, selecting the save icon on any trail will only fill the icon for the first trail displayed, which I did some research on solutions for, and will continue to work on later. I edited saved.html to display a message when a logged in user has no saved trails informing them of that. I then started researching ways to get the trail data necessary to upload notes for a specific trail when the user clicks the save button. This is difficult because the trails are displayed with a for loop, and therefore do not have unique IDs to get them from the HTML by. I spent some time trying to set the save buttons to give them an ID name that matches the trail name to use that for updating the database.</t>
+    <t xml:space="preserve">I moved the main.js file to the static folder, and the terminal no longer throws a 404 when trying to load it. However, the JS function still did not execute, so I spent some time researching and debugging that issue. I eventually found that the JavaScript file was including the full domain as the image source (starting with http://(my domain), and changed the if statement to check if the source ended with the file path, rather than if it was equal to it, which fixed the issue. However, selecting the save icon on any trail will only fill the icon for the first trail displayed, which I did some research on solutions for, and will continue to work on later. I edited saved.html to display a message informing a logged in user if they have no saved trails. I then started researching ways to get the trail data necessary to upload notes for a specific trail when the user clicks the save button. This was difficult because the trails are displayed with a for loop, and therefore didn’t initially have unique IDs to get them from the HTML by. After a lot of research and trial and error, I eventually got the IDs to be dynamically assigned to match the trail ID by giving them placeholder IDs that would then be updated by a JavaScript function within the for loop, so they can be grabbed by a separate function then passed to Python, where they can be used to update the database. I created the saveNotes function in main.js to accomplish this. I wanted to switch to a similar system for the notes input itself, and while changing it from a FlaskWTF system to standard HTML that could also have its ID edited via JavaScript, I was able to fix the issue of the notes text not auto-populating the entry box. I then set up the saveNotes function to get the entered notes as well, and pass that, along with the trail ID, to a new function in main.py called save_notes. I set this function up to take the ID, query for it in the notes table, and update the user’s note accordingly. I then added an alert in the saveNotes function in main.js to notify the user that their note had been saved. Finally for today, I changed the tagline on the home page from “spend less time searching and more time riding” to “less searching, more riding”, thanks to the suggestion of my girlfriend who knows much more about marketing than I do and said it would sound punchier. </t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -618,6 +618,12 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -709,7 +715,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -806,6 +812,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,9 +899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>226440</xdr:colOff>
+      <xdr:colOff>226080</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -901,7 +911,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6579000" cy="5046120"/>
+          <a:ext cx="6578640" cy="5045760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1112,9 +1122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>163800</xdr:colOff>
+      <xdr:colOff>163440</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>179640</xdr:rowOff>
+      <xdr:rowOff>179280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1124,7 +1134,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2558880" cy="708840"/>
+          <a:ext cx="2558520" cy="708480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1191,9 +1201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>65160</xdr:colOff>
+      <xdr:colOff>64800</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1203,7 +1213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3719160" cy="15635880"/>
+          <a:ext cx="3718800" cy="15635520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1306,9 +1316,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>576720</xdr:colOff>
+      <xdr:colOff>576360</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1318,7 +1328,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3952080" cy="17456040"/>
+          <a:ext cx="3951720" cy="17455680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1565,9 +1575,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>84600</xdr:colOff>
+      <xdr:colOff>84240</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1577,7 +1587,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3504240" cy="15489360"/>
+          <a:ext cx="3503880" cy="15489000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3180,7 +3190,7 @@
   <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3663,7 +3673,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" customFormat="false" ht="266.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="531.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
         <v>156</v>
       </c>
@@ -3671,12 +3681,12 @@
         <v>45995</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>1.75</v>
+        <v>3.5</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="24" t="s">
         <v>157</v>
       </c>
       <c r="F27" s="12"/>

</xml_diff>

<commit_message>
Partial commit for today.
</commit_message>
<xml_diff>
--- a/project_tracker_workbook.xlsx
+++ b/project_tracker_workbook.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="159">
   <si>
     <t xml:space="preserve">Team Members</t>
   </si>
@@ -529,6 +529,9 @@
   <si>
     <t xml:space="preserve">I moved the main.js file to the static folder, and the terminal no longer throws a 404 when trying to load it. However, the JS function still did not execute, so I spent some time researching and debugging that issue. I eventually found that the JavaScript file was including the full domain as the image source (starting with http://(my domain), and changed the if statement to check if the source ended with the file path, rather than if it was equal to it, which fixed the issue. However, selecting the save icon on any trail will only fill the icon for the first trail displayed, which I did some research on solutions for, and will continue to work on later. I edited saved.html to display a message informing a logged in user if they have no saved trails. I then started researching ways to get the trail data necessary to upload notes for a specific trail when the user clicks the save button. This was difficult because the trails are displayed with a for loop, and therefore didn’t initially have unique IDs to get them from the HTML by. After a lot of research and trial and error, I eventually got the IDs to be dynamically assigned to match the trail ID by giving them placeholder IDs that would then be updated by a JavaScript function within the for loop, so they can be grabbed by a separate function then passed to Python, where they can be used to update the database. I created the saveNotes function in main.js to accomplish this. I wanted to switch to a similar system for the notes input itself, and while changing it from a FlaskWTF system to standard HTML that could also have its ID edited via JavaScript, I was able to fix the issue of the notes text not auto-populating the entry box. I then set up the saveNotes function to get the entered notes as well, and pass that, along with the trail ID, to a new function in main.py called save_notes. I set this function up to take the ID, query for it in the notes table, and update the user’s note accordingly. I then added an alert in the saveNotes function in main.js to notify the user that their note had been saved. Finally for today, I changed the tagline on the home page from “spend less time searching and more time riding” to “less searching, more riding”, thanks to the suggestion of my girlfriend who knows much more about marketing than I do and said it would sound punchier. </t>
   </si>
+  <si>
+    <t xml:space="preserve">I changed how the save button is identified by the fillMark function in main.js to solve the issue of the correct bookmark not filling when being clicked. I then set up the function to pass data to a function I created in main.py called save_trail so it could handle updating the database. I then edited results.html to only show the save button if there is a user logged in. After that, I finished setting up save_trail to add or remove a trail from the user’s saved trails in the notes table when the bookmark is selected or deselected, respectively. </t>
+  </si>
 </sst>
 </file>
 
@@ -538,7 +541,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -618,12 +621,6 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -715,7 +712,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -812,10 +809,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,9 +892,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>226080</xdr:colOff>
+      <xdr:colOff>225720</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -911,7 +904,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276120" y="270000"/>
-          <a:ext cx="6578640" cy="5045760"/>
+          <a:ext cx="6578280" cy="5045400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1122,9 +1115,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>163440</xdr:colOff>
+      <xdr:colOff>163080</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>179280</xdr:rowOff>
+      <xdr:rowOff>178920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1134,7 +1127,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4725000" y="207360"/>
-          <a:ext cx="2558520" cy="708480"/>
+          <a:ext cx="2558160" cy="708120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1201,9 +1194,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>64800</xdr:colOff>
+      <xdr:colOff>64440</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1213,7 +1206,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7090920" y="177120"/>
-          <a:ext cx="3718800" cy="15635520"/>
+          <a:ext cx="3718440" cy="15635160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1316,9 +1309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>576360</xdr:colOff>
+      <xdr:colOff>576000</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1328,7 +1321,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9739800" y="300960"/>
-          <a:ext cx="3951720" cy="17455680"/>
+          <a:ext cx="3951360" cy="17455320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1575,9 +1568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>84240</xdr:colOff>
+      <xdr:colOff>83880</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1587,7 +1580,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8812440" y="217080"/>
-          <a:ext cx="3503880" cy="15489000"/>
+          <a:ext cx="3503520" cy="15488640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3189,8 +3182,8 @@
   </sheetPr>
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3686,19 +3679,25 @@
       <c r="D27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="12" t="s">
         <v>157</v>
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="128.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="12"/>
+      <c r="B28" s="22" t="n">
+        <v>45996</v>
+      </c>
+      <c r="C28" s="12" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D28" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="F28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>